<commit_message>
add battery to spreadsheet
</commit_message>
<xml_diff>
--- a/design_documents/design.xlsx
+++ b/design_documents/design.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/74db7c87a9029f2a/Documents/PCB/SmallFlight1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/74db7c87a9029f2a/Documents/PCB/SmallFlight1/design_documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="364" documentId="11_F25DC773A252ABDACC1048E409DB493A5ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{63C0DE87-38A7-4B5C-B76B-07491D3C1D10}"/>
+  <xr:revisionPtr revIDLastSave="414" documentId="11_F25DC773A252ABDACC1048E409DB493A5ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{21680C95-C6F3-4C46-8055-2EF0D984F5D1}"/>
   <bookViews>
-    <workbookView xWindow="11865" yWindow="2055" windowWidth="16155" windowHeight="10935" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6780" yWindow="1575" windowWidth="21240" windowHeight="11415" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ideation" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="80">
   <si>
     <t xml:space="preserve">Estimated Flight Profile </t>
   </si>
@@ -257,6 +257,27 @@
   </si>
   <si>
     <t xml:space="preserve"> Part Selection</t>
+  </si>
+  <si>
+    <t>Polymer Lithium Ion Battery (LiPo) 3.7V 400mAh</t>
+  </si>
+  <si>
+    <t>Polymer Lithium Ion Battery (LiPo) 3.7V 1100mAh</t>
+  </si>
+  <si>
+    <t>https://core-electronics.com.au/polymer-lithium-ion-battery-400mah-38456.html</t>
+  </si>
+  <si>
+    <t>https://core-electronics.com.au/polymer-lithium-ion-battery-1000mah-38458.html</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Current (mAh)</t>
   </si>
 </sst>
 </file>
@@ -332,7 +353,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -353,6 +374,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -639,7 +666,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="E3" sqref="E3:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -807,7 +834,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E9"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -976,19 +1003,24 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1B774BC-19AE-4085-853D-BC5D7AB716CB}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.140625" customWidth="1"/>
+    <col min="9" max="9" width="45.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="76.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>71</v>
       </c>
@@ -999,7 +1031,7 @@
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>33</v>
       </c>
@@ -1013,8 +1045,23 @@
       </c>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I2" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
       <c r="B3" s="3" t="s">
         <v>65</v>
@@ -1034,8 +1081,23 @@
       <c r="G3" s="3" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I3" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="J3" s="8">
+        <v>3.7</v>
+      </c>
+      <c r="K3" s="8">
+        <v>400</v>
+      </c>
+      <c r="L3" s="8">
+        <v>1</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>34</v>
       </c>
@@ -1057,8 +1119,23 @@
       <c r="G4" s="2">
         <v>240</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I4" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="J4" s="8">
+        <v>3.7</v>
+      </c>
+      <c r="K4" s="8">
+        <v>1100</v>
+      </c>
+      <c r="L4" s="8">
+        <v>2</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>36</v>
       </c>
@@ -1081,7 +1158,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>1040310811</v>
       </c>
@@ -1104,7 +1181,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>61</v>
       </c>
@@ -1127,7 +1204,7 @@
         <v>3.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>35</v>
       </c>
@@ -1150,7 +1227,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>41</v>
       </c>
@@ -1173,7 +1250,7 @@
         <v>1130</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>56</v>
       </c>

</xml_diff>